<commit_message>
Add sig levels and XAdES section
</commit_message>
<xml_diff>
--- a/docs/assets/AdESFormats.xlsx
+++ b/docs/assets/AdESFormats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\DigitalSignature\docs\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550281E2-C9D5-4848-AAC9-C37614828CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38399C4E-8BAC-4285-AFE1-E1209EED4F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31140" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{E64B6A7A-4BEE-4A1D-AD08-7FB226B75D19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="26">
   <si>
     <t>XML</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Protupotpis</t>
-  </si>
-  <si>
-    <t>Samostalni vremenski žig</t>
   </si>
   <si>
     <t>Profil potipsa</t>
@@ -184,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -286,13 +283,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -310,7 +307,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -319,52 +316,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -379,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -408,40 +360,31 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -758,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4268C03A-431C-4239-87FA-5B564E4CA041}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection sqref="A1:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,12 +718,11 @@
     <col min="7" max="8" width="7.7109375" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5">
+    <row r="1" spans="1:11" ht="25.5">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -808,463 +750,421 @@
       <c r="K1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="25.5">
-      <c r="A2" s="11" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="25.5">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="25.5">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="J3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="25.5">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="J5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="51">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25.5">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="25.5">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="J9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25.5">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="25.5">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="25.5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="38.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="J11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="25.5">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="25.5">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="25.5">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="25.5">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1">
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="1"/>
@@ -1276,9 +1176,8 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="1"/>
@@ -1290,9 +1189,8 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1"/>
@@ -1304,9 +1202,8 @@
       <c r="I17" s="3"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
@@ -1318,9 +1215,8 @@
       <c r="I18" s="1"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="1"/>
@@ -1332,9 +1228,8 @@
       <c r="I19" s="1"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1"/>
@@ -1346,9 +1241,8 @@
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1">
       <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1360,9 +1254,8 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1374,7 +1267,6 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>